<commit_message>
get working DF for 2009 data
</commit_message>
<xml_diff>
--- a/AllStudentsWithNumbers.xlsx
+++ b/AllStudentsWithNumbers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/travisallen/Desktop/CornellTech/Spring2018/Practicum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/travisallen/Desktop/CornellTech/Spring2018/Practicum/Practica/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="754">
   <si>
     <t>Adler, Karen</t>
   </si>
@@ -2286,9 +2286,6 @@
   </si>
   <si>
     <t>Zyburo, Dara</t>
-  </si>
-  <si>
-    <t>P/F</t>
   </si>
   <si>
     <t>Year</t>
@@ -2342,207 +2339,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -2826,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D850"/>
+  <dimension ref="A1:C850"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2838,21 +2635,18 @@
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +2657,7 @@
         <v>865413</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2874,7 +2668,7 @@
         <v>367062</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2885,7 +2679,7 @@
         <v>245385</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2896,7 +2690,7 @@
         <v>286071</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2907,7 +2701,7 @@
         <v>536349</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2918,7 +2712,7 @@
         <v>183678</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2929,7 +2723,7 @@
         <v>767012</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2940,7 +2734,7 @@
         <v>787746</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2951,7 +2745,7 @@
         <v>526528</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2962,7 +2756,7 @@
         <v>172459</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2973,7 +2767,7 @@
         <v>644930</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2984,7 +2778,7 @@
         <v>739271</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2995,7 +2789,7 @@
         <v>210135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3006,7 +2800,7 @@
         <v>370581</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -12193,7 +11987,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF(A:C, A1)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>